<commit_message>
Updated the last survey results
</commit_message>
<xml_diff>
--- a/survey-3/survey-3-report.xlsx
+++ b/survey-3/survey-3-report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaron/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79390DE3-F799-8A4A-97E9-6FDCB613F7E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43CAC454-6EC7-D54D-8127-788B74BFE02E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11740" yWindow="-23180" windowWidth="24960" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4440" yWindow="740" windowWidth="24960" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Data" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1800" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2025" uniqueCount="23">
   <si>
     <t>Click to see the commitCommit Message 1:Refactor: Improve resource handling in writeSnapshotManifest methodThis commit refactors the `writeSnapshotManifest` method in the `ColumnFamilyStore.java` file. The changes involve the use of a try-with-resources statement to ensure that the `PrintStream` object is properly closed after use. This improves the resource handling in the method and makes the code more robust and easier to maintain.Commit Message 2:Refactor: Refactor writeSnapshotManifest method to use try-with-resources statementThe writeSnapshotManifest method has been refactored to use a try-with-resources statement to automatically close the PrintStream object. This change improves code style and reduces the risk of resource leaks. The method's functionality remains the same, and it still writes the snapshot manifest file with the given snapshot name and files array. Please select the superior commit message in each evaluation criterion. </t>
   </si>
@@ -473,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:BW24"/>
+  <dimension ref="A1:BW27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="BX1" sqref="BX1:BY1048576"/>
+    <sheetView tabSelected="1" topLeftCell="BK1" workbookViewId="0">
+      <selection activeCell="CB11" sqref="CB11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5929,6 +5929,687 @@
         <v>21</v>
       </c>
     </row>
+    <row r="25" spans="1:75" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="P25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="R25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="T25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="U25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="V25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="W25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="X25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AC25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AD25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AE25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AF25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AG25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AH25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AI25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AJ25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AK25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AL25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AM25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AN25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AO25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AP25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AQ25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AR25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AS25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AT25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AU25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AV25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AW25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AX25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AY25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AZ25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="BA25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="BB25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="BC25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="BD25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="BE25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="BF25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="BG25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="BH25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="BI25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="BJ25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="BK25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="BL25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="BM25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="BN25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="BO25" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="BP25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="BQ25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="BR25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="BS25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="BT25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="BU25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="BV25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="BW25" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:75" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="O26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="P26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="R26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="T26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="U26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="V26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="W26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="X26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Y26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AA26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AC26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AD26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AG26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AH26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AI26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AJ26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AK26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AL26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AM26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AN26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AO26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AP26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AQ26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AR26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AS26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AT26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AU26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AV26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AW26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AX26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AY26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AZ26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="BA26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="BB26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="BC26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="BD26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="BE26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="BF26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="BG26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="BH26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="BI26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="BJ26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="BK26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="BL26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="BM26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="BN26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="BO26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="BP26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="BQ26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="BR26" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="BS26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="BT26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="BU26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="BV26" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="BW26" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:75" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="R27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="S27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="T27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="U27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="V27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="W27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="X27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Y27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AA27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AC27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AD27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AF27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AG27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AH27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AI27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AJ27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AK27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AL27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AM27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AN27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AO27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AP27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AQ27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AR27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AS27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AT27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AU27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AV27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AW27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AX27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AY27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AZ27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="BA27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="BB27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="BC27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="BD27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="BE27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="BF27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="BG27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="BH27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="BI27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="BJ27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="BK27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="BL27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="BM27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="BN27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="BO27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="BP27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="BQ27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="BR27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="BS27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="BT27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="BU27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="BV27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="BW27" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Correcting the survey report for survey 3
</commit_message>
<xml_diff>
--- a/survey-3/survey-3-report.xlsx
+++ b/survey-3/survey-3-report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aaron/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43CAC454-6EC7-D54D-8127-788B74BFE02E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79390DE3-F799-8A4A-97E9-6FDCB613F7E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="740" windowWidth="24960" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11740" yWindow="-23180" windowWidth="24960" windowHeight="18380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw Data" sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2025" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1800" uniqueCount="23">
   <si>
     <t>Click to see the commitCommit Message 1:Refactor: Improve resource handling in writeSnapshotManifest methodThis commit refactors the `writeSnapshotManifest` method in the `ColumnFamilyStore.java` file. The changes involve the use of a try-with-resources statement to ensure that the `PrintStream` object is properly closed after use. This improves the resource handling in the method and makes the code more robust and easier to maintain.Commit Message 2:Refactor: Refactor writeSnapshotManifest method to use try-with-resources statementThe writeSnapshotManifest method has been refactored to use a try-with-resources statement to automatically close the PrintStream object. This change improves code style and reduces the risk of resource leaks. The method's functionality remains the same, and it still writes the snapshot manifest file with the given snapshot name and files array. Please select the superior commit message in each evaluation criterion. </t>
   </si>
@@ -473,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:BW27"/>
+  <dimension ref="A1:BW24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BK1" workbookViewId="0">
-      <selection activeCell="CB11" sqref="CB11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="BX1" sqref="BX1:BY1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5929,687 +5929,6 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:75" x14ac:dyDescent="0.2">
-      <c r="A25" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K25" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="L25" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="M25" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="N25" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="O25" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="P25" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q25" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="R25" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="S25" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="T25" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="U25" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="V25" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="W25" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="X25" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y25" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z25" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AA25" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="AB25" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AC25" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AD25" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="AE25" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AF25" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="AG25" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="AH25" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AI25" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AJ25" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AK25" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="AL25" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AM25" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="AN25" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AO25" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="AP25" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="AQ25" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="AR25" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="AS25" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="AT25" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AU25" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="AV25" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AW25" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AX25" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AY25" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="AZ25" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="BA25" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="BB25" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="BC25" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="BD25" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="BE25" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="BF25" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="BG25" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="BH25" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="BI25" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="BJ25" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="BK25" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="BL25" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="BM25" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="BN25" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="BO25" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="BP25" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="BQ25" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="BR25" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="BS25" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="BT25" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="BU25" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="BV25" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="BW25" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="1:75" x14ac:dyDescent="0.2">
-      <c r="A26" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I26" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J26" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K26" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L26" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="M26" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="N26" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="O26" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="P26" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q26" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="R26" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="S26" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="T26" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="U26" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="V26" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="W26" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="X26" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="Y26" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="Z26" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA26" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="AB26" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AC26" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="AD26" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AE26" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="AF26" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="AG26" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="AH26" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="AI26" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="AJ26" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="AK26" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="AL26" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AM26" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="AN26" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AO26" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="AP26" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="AQ26" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="AR26" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="AS26" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="AT26" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AU26" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="AV26" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AW26" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AX26" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AY26" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AZ26" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="BA26" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="BB26" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="BC26" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="BD26" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="BE26" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="BF26" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="BG26" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="BH26" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="BI26" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="BJ26" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="BK26" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="BL26" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="BM26" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="BN26" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="BO26" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="BP26" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="BQ26" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="BR26" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="BS26" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="BT26" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="BU26" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="BV26" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="BW26" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="1:75" x14ac:dyDescent="0.2">
-      <c r="A27" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="K27" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L27" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="M27" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="N27" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="O27" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="P27" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q27" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="R27" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="S27" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="T27" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="U27" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="V27" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="W27" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="X27" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Y27" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Z27" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AA27" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="AB27" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AC27" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="AD27" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AE27" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="AF27" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AG27" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="AH27" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="AI27" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="AJ27" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="AK27" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="AL27" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AM27" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="AN27" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="AO27" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="AP27" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AQ27" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="AR27" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="AS27" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="AT27" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AU27" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AV27" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AW27" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AX27" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="AY27" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="AZ27" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="BA27" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="BB27" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="BC27" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="BD27" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="BE27" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="BF27" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="BG27" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="BH27" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="BI27" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="BJ27" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="BK27" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="BL27" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="BM27" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="BN27" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="BO27" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="BP27" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="BQ27" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="BR27" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="BS27" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="BT27" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="BU27" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="BV27" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="BW27" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>